<commit_message>
running with full data
Updated dates columns to 4 digit years in “data” and “log”

updating script to run with full data (plots, na.rm’s, etc)
</commit_message>
<xml_diff>
--- a/2015_MMMILC_dataCleaningLog.xlsx
+++ b/2015_MMMILC_dataCleaningLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="6600" yWindow="840" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2015_MMMILC_dataCleaningLog.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t>obs.IDs</t>
   </si>
@@ -30,12 +30,6 @@
     <t>action.taken</t>
   </si>
   <si>
-    <t>no observation ID</t>
-  </si>
-  <si>
-    <t>ID's 1-58 added</t>
-  </si>
-  <si>
     <t>any observations with NE, DEAD, MISSING status (ex 74)</t>
   </si>
   <si>
@@ -228,24 +222,12 @@
     <t>all data missing (except milkweed ID)</t>
   </si>
   <si>
-    <t>observation ID added, all other data left blank</t>
-  </si>
-  <si>
     <t>stage.length "1st instar(0.9mm)"</t>
   </si>
   <si>
     <t>changed to 1L-0.9</t>
   </si>
   <si>
-    <t>3240-3246</t>
-  </si>
-  <si>
-    <t>obs id missing</t>
-  </si>
-  <si>
-    <t>obs id added</t>
-  </si>
-  <si>
     <t>stage.length "nond"</t>
   </si>
   <si>
@@ -393,7 +375,7 @@
     <t>commas added</t>
   </si>
   <si>
-    <t>1-58</t>
+    <t>None - left blank</t>
   </si>
 </sst>
 </file>
@@ -429,10 +411,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,55 +770,55 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>124</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -848,26 +829,26 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>22</v>
+      <c r="A9">
+        <v>295</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -877,30 +858,30 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10">
-        <v>295</v>
+      <c r="A10" t="s">
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>28</v>
+      <c r="A12" s="1">
+        <v>10341036</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -910,19 +891,19 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>10341036</v>
+      <c r="A13" t="s">
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>33</v>
+      <c r="A14">
+        <v>1592</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -932,63 +913,63 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15">
-        <v>1592</v>
+      <c r="A15" t="s">
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>1743</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17">
-        <v>1743</v>
+      <c r="A17" t="s">
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>47</v>
+      <c r="A20">
+        <v>2052</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
@@ -999,7 +980,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>2052</v>
+        <v>2127</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
@@ -1010,7 +991,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>2127</v>
+        <v>2656</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
@@ -1021,7 +1002,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>2656</v>
+        <v>2743</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
@@ -1032,7 +1013,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>2743</v>
+        <v>2759</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
@@ -1043,7 +1024,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>2759</v>
+        <v>2875</v>
       </c>
       <c r="B25" t="s">
         <v>58</v>
@@ -1054,7 +1035,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>2875</v>
+        <v>3030</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -1064,217 +1045,217 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27">
-        <v>3030</v>
+      <c r="A27" t="s">
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="A29">
+        <v>3219</v>
+      </c>
+      <c r="B29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>3219</v>
+        <v>3329</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>3500</v>
+      </c>
+      <c r="B31" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>3329</v>
+        <v>3765</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>3500</v>
+        <v>3937</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>3765</v>
+        <v>4030</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>3937</v>
+        <v>4066</v>
       </c>
       <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>81</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B36" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36">
-        <v>4030</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>4066</v>
+        <v>4235</v>
       </c>
       <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
         <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
         <v>87</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>4235</v>
+        <v>4553</v>
       </c>
       <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
         <v>90</v>
-      </c>
-      <c r="C39" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
         <v>92</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>4553</v>
+        <v>4707</v>
       </c>
       <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
         <v>95</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>4772</v>
+      </c>
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
         <v>97</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>98</v>
       </c>
-      <c r="C42" t="s">
+      <c r="B43" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43">
-        <v>4707</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>100</v>
-      </c>
-      <c r="C43" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>4772</v>
+        <v>4920</v>
       </c>
       <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
         <v>102</v>
-      </c>
-      <c r="C44" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
         <v>104</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>105</v>
       </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46">
-        <v>4920</v>
       </c>
       <c r="B46" t="s">
         <v>107</v>
@@ -1284,69 +1265,47 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" t="s">
+      <c r="A47">
+        <v>5624</v>
+      </c>
+      <c r="B47" t="s">
         <v>109</v>
       </c>
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>113</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B49" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
-        <v>5624</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>115</v>
       </c>
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
+      <c r="A50">
+        <v>6000</v>
+      </c>
+      <c r="B50" t="s">
         <v>116</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>117</v>
-      </c>
-      <c r="C50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <v>6000</v>
-      </c>
-      <c r="B52" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of meeting 1/14
added list of to-dos within script

added annotated unentered data pdf
</commit_message>
<xml_diff>
--- a/2015_MMMILC_dataCleaningLog.xlsx
+++ b/2015_MMMILC_dataCleaningLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1700" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14680" yWindow="460" windowWidth="27920" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2015_MMMILC_dataCleaningLog.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
   <si>
     <t>obs.IDs</t>
   </si>
@@ -48,15 +48,6 @@
     <t xml:space="preserve">None - assume stem length list is correct. count stems over 5 cm in analysis script and replace stem count when number is higher </t>
   </si>
   <si>
-    <t>any observations with MORE stems than listed in stem lengths columns (ex 110)</t>
-  </si>
-  <si>
-    <t>some plants with 11+ stems, or typos in stem.count</t>
-  </si>
-  <si>
-    <t>None - assume stem length list is correct. count stems over 5 cm in analysis script and replace stem count except when stemcount is larger than 10</t>
-  </si>
-  <si>
     <t>137, 138, 139, 141</t>
   </si>
   <si>
@@ -388,6 +379,21 @@
   </si>
   <si>
     <t>changed to L-0.9</t>
+  </si>
+  <si>
+    <t>CHECK INDIVS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>4716, 4718, 5603</t>
+  </si>
+  <si>
+    <t>dates incorrect (typos)</t>
+  </si>
+  <si>
+    <t>fixed typos</t>
   </si>
 </sst>
 </file>
@@ -757,15 +763,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
     <col min="2" max="2" width="78.5" customWidth="1"/>
     <col min="3" max="3" width="66.83203125" customWidth="1"/>
   </cols>
@@ -786,10 +792,10 @@
         <v>295</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -797,10 +803,10 @@
         <v>1592</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -808,10 +814,10 @@
         <v>1743</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -819,10 +825,10 @@
         <v>2052</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -830,10 +836,10 @@
         <v>2127</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -841,10 +847,10 @@
         <v>2656</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -852,10 +858,10 @@
         <v>2743</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -863,10 +869,10 @@
         <v>2759</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -874,10 +880,10 @@
         <v>2875</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -885,10 +891,10 @@
         <v>3030</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -896,10 +902,10 @@
         <v>3219</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -907,10 +913,10 @@
         <v>3500</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -918,10 +924,10 @@
         <v>3574</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -929,10 +935,10 @@
         <v>3765</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -940,10 +946,10 @@
         <v>3932</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -951,10 +957,10 @@
         <v>3937</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -962,10 +968,10 @@
         <v>4030</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -973,10 +979,10 @@
         <v>4066</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -984,10 +990,10 @@
         <v>4235</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -995,10 +1001,10 @@
         <v>4553</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1006,10 +1012,10 @@
         <v>4707</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1017,10 +1023,10 @@
         <v>4772</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1028,10 +1034,10 @@
         <v>4920</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1039,10 +1045,10 @@
         <v>5624</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1050,10 +1056,10 @@
         <v>6000</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1061,233 +1067,236 @@
         <v>10341036</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>100</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>104</v>
       </c>
-      <c r="C42" t="s">
+      <c r="B43" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>107</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>108</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
         <v>13</v>
       </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1298,48 +1307,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data cleaning log
</commit_message>
<xml_diff>
--- a/2015_MMMILC_dataCleaningLog.xlsx
+++ b/2015_MMMILC_dataCleaningLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="460" windowWidth="27920" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="15140" yWindow="4080" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2015_MMMILC_dataCleaningLog.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
   <si>
     <t>obs.IDs</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>fixed typos</t>
+  </si>
+  <si>
+    <t>stage.length 5mm</t>
+  </si>
+  <si>
+    <t>changed to L1-5, because L1 most likely</t>
   </si>
 </sst>
 </file>
@@ -763,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1354,6 +1360,17 @@
         <v>124</v>
       </c>
     </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>7945</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C52">
     <sortCondition ref="A2:A52"/>

</xml_diff>